<commit_message>
sistemata larghezza colonne che era saltata, tolto commento tra parentesi
</commit_message>
<xml_diff>
--- a/Documents/Verifiche documenti.xlsx
+++ b/Documents/Verifiche documenti.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Documents\GitHub\Leaf\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Davide/Desktop/GitHub/Leaf/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="705" yWindow="465" windowWidth="19245" windowHeight="11505"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="19240" windowHeight="11500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PQ</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>AR</t>
-  </si>
-  <si>
-    <t>39(contando parole senza g)</t>
   </si>
   <si>
     <t>Periodi troppo lunghi o complessi</t>
@@ -128,7 +125,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -411,22 +410,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -446,9 +443,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -457,9 +454,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -468,9 +465,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -479,9 +476,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -490,14 +487,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -506,9 +503,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -517,34 +514,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>13</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
       </c>
       <c r="B10">
         <v>16</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E11" s="1">
         <v>2.0152777777777802</v>

</xml_diff>

<commit_message>
aggiunti valori della verifica sul PdP
</commit_message>
<xml_diff>
--- a/Documents/Verifiche documenti.xlsx
+++ b/Documents/Verifiche documenti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="19240" windowHeight="11500"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="24620" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>PQ</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>126.30</t>
+  </si>
+  <si>
+    <t>// Cella E10: Marco, dovresti spostare gli errori che dicevi delle parole a cui manca la 'g' a pedice in 'Violazioni delle norme tipografiche'</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -128,6 +131,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -408,17 +412,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.83203125" customWidth="1"/>
     <col min="2" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="5" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
@@ -450,6 +455,9 @@
       <c r="B2">
         <v>2</v>
       </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
@@ -461,6 +469,9 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
       <c r="E3">
         <v>4</v>
       </c>
@@ -472,6 +483,9 @@
       <c r="B4">
         <v>6</v>
       </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
       <c r="E4">
         <v>0</v>
       </c>
@@ -483,6 +497,9 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
       <c r="E5">
         <v>0</v>
       </c>
@@ -491,6 +508,9 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="C6">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -499,6 +519,9 @@
       <c r="B7">
         <v>0</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="E7">
         <v>6</v>
       </c>
@@ -510,6 +533,9 @@
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="E8">
         <v>6</v>
       </c>
@@ -521,6 +547,9 @@
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
       <c r="E9">
         <v>0</v>
       </c>
@@ -532,6 +561,9 @@
       <c r="B10">
         <v>16</v>
       </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
       <c r="E10" s="2">
         <v>39</v>
       </c>
@@ -547,7 +579,15 @@
         <v>2.0152777777777802</v>
       </c>
     </row>
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:XFD13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Aggiunti dati verifica delle NP su verifica documenti
</commit_message>
<xml_diff>
--- a/Documents/Verifiche documenti.xlsx
+++ b/Documents/Verifiche documenti.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Davide/Desktop/GitHub/Leaf/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="24620" windowHeight="15540"/>
+    <workbookView xWindow="705" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="124519" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>PQ</t>
   </si>
@@ -78,16 +73,19 @@
   </si>
   <si>
     <t>// Cella E10: Marco, dovresti spostare gli errori che dicevi delle parole a cui manca la 'g' a pedice in 'Violazioni delle norme tipografiche'</t>
+  </si>
+  <si>
+    <t>51.54</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -100,6 +98,14 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -132,6 +138,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -192,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -227,7 +234,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -404,31 +411,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" customWidth="1"/>
-    <col min="2" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -448,7 +455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -458,11 +465,14 @@
       <c r="C2">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -472,11 +482,14 @@
       <c r="C3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -486,11 +499,14 @@
       <c r="C4">
         <v>4</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -500,19 +516,25 @@
       <c r="C5">
         <v>13</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="C6">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -520,13 +542,16 @@
         <v>0</v>
       </c>
       <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -534,13 +559,16 @@
         <v>0</v>
       </c>
       <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -550,11 +578,14 @@
       <c r="C9">
         <v>21</v>
       </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -564,22 +595,28 @@
       <c r="C10">
         <v>6</v>
       </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
       <c r="E10" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D11" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E11" s="1">
         <v>2.0152777777777802</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="4" customFormat="1">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -589,6 +626,6 @@
     <mergeCell ref="A13:XFD13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aggiunti i valori della verifica al glossario
</commit_message>
<xml_diff>
--- a/Documents/Verifiche documenti.xlsx
+++ b/Documents/Verifiche documenti.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Davide/Desktop/GitHub/Leaf/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="705" yWindow="465" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="20740" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -72,20 +77,20 @@
     <t>126.30</t>
   </si>
   <si>
-    <t>// Cella E10: Marco, dovresti spostare gli errori che dicevi delle parole a cui manca la 'g' a pedice in 'Violazioni delle norme tipografiche'</t>
-  </si>
-  <si>
     <t>51.54</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -98,14 +103,6 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,15 +127,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -411,51 +412,51 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -471,8 +472,12 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -488,8 +493,12 @@
       <c r="E3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -505,8 +514,12 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -522,19 +535,33 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
       <c r="C6">
         <v>38</v>
       </c>
       <c r="D6">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="E6">
+        <v>37</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -550,8 +577,12 @@
       <c r="E7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -567,8 +598,12 @@
       <c r="E8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -584,13 +619,17 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -598,33 +637,33 @@
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="1">
-        <v>2.0152777777777802</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="4" customFormat="1">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A13:XFD13"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiunti valore indice Gulpease
</commit_message>
<xml_diff>
--- a/Documents/Verifiche documenti.xlsx
+++ b/Documents/Verifiche documenti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="20740" windowHeight="11760"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>PQ</t>
   </si>
@@ -72,24 +72,12 @@
   </si>
   <si>
     <t>Violazioni delle norme tipografiche</t>
-  </si>
-  <si>
-    <t>126.30</t>
-  </si>
-  <si>
-    <t>51.54</t>
-  </si>
-  <si>
-    <t>158.53</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,10 +122,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -423,7 +411,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -649,18 +637,22 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1"/>
+      <c r="B11" s="4">
+        <v>51</v>
+      </c>
+      <c r="C11" s="4">
+        <v>54</v>
+      </c>
+      <c r="D11" s="5">
+        <v>60</v>
+      </c>
+      <c r="E11" s="4">
+        <v>55</v>
+      </c>
+      <c r="F11" s="4">
+        <v>67</v>
+      </c>
+      <c r="G11" s="4"/>
     </row>
     <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
aggiunto valore gulpease AR
</commit_message>
<xml_diff>
--- a/Documents/Verifiche documenti.xlsx
+++ b/Documents/Verifiche documenti.xlsx
@@ -411,7 +411,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -568,7 +568,9 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -589,7 +591,9 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -652,7 +656,9 @@
       <c r="F11" s="4">
         <v>67</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
inseriti valori della verifica dell'AR
</commit_message>
<xml_diff>
--- a/Documents/Verifiche documenti.xlsx
+++ b/Documents/Verifiche documenti.xlsx
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -424,7 +424,7 @@
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -444,7 +444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -463,9 +463,15 @@
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>SUM(B2+E2+F2+G2,C2+D2)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -484,9 +490,15 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>SUM(B3+C3+D3+E3+F3+G3)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -505,9 +517,15 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <f>SUM(B4+C4+D4+E4+F4+G4)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -526,9 +544,15 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f>SUM(B5+C5+D5+E5+F5+G5)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -547,9 +571,15 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f>SUM(B6+C6+D6+E6+F6+G6)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -571,8 +601,11 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -594,8 +627,11 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -614,9 +650,15 @@
       <c r="F9">
         <v>6</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <f>SUM(B9+C9+D9+E9+F9+G9)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -635,32 +677,42 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>SUM(B10+C10+D10+E10+F10+G10)</f>
         <v>14</v>
       </c>
-      <c r="B11" s="4">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4">
         <v>51</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C12" s="4">
         <v>54</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D12" s="5">
         <v>60</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E12" s="4">
         <v>55</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F12" s="4">
         <v>67</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G12" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
aggiornato appendice resoconto PQ con dati delle verifiche
</commit_message>
<xml_diff>
--- a/Documents/Verifiche documenti.xlsx
+++ b/Documents/Verifiche documenti.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -411,7 +411,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>